<commit_message>
Fichier cas de tests utilisateurs complétés
</commit_message>
<xml_diff>
--- a/Tests/Plan_de_test_horaire.xlsx
+++ b/Tests/Plan_de_test_horaire.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Cegep\CegepSth\6_Session\PP\Gestion stagiaires SPU\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E06A3708-3BD1-4359-BF44-C30A66B75D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12140E30-217E-436A-9EE6-185E6EF1C1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{41F3187D-F1A2-49DE-9E3A-08B0683190F9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{41F3187D-F1A2-49DE-9E3A-08B0683190F9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Horaire" sheetId="1" r:id="rId1"/>
+    <sheet name="Horaire" sheetId="3" r:id="rId1"/>
+    <sheet name="Utilisateur" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>Tests</t>
   </si>
@@ -92,6 +93,174 @@
   </si>
   <si>
     <t>Ajouter une seule plage horaire qui est déjà prise.</t>
+  </si>
+  <si>
+    <t>Se connecter, stagiaire</t>
+  </si>
+  <si>
+    <t>Redirection vers la page d'accueil</t>
+  </si>
+  <si>
+    <t>Redirection vers la page d'accueil avec succès</t>
+  </si>
+  <si>
+    <t>Se connecter, coordonateur</t>
+  </si>
+  <si>
+    <t>Se connecter, maître de stage</t>
+  </si>
+  <si>
+    <t>Se connecter, employeur</t>
+  </si>
+  <si>
+    <t>Se connecter, enseignant</t>
+  </si>
+  <si>
+    <t>Redirection vers la page de gestion des utilisateurs</t>
+  </si>
+  <si>
+    <t>Redirection vers la page de gestion des utilisateurs avec succès</t>
+  </si>
+  <si>
+    <t>Redirection vers la page de gestion des maîtres de stages</t>
+  </si>
+  <si>
+    <t>Échec</t>
+  </si>
+  <si>
+    <t>Pas encore implémentée</t>
+  </si>
+  <si>
+    <t>Entrer les bonnes données de connexion</t>
+  </si>
+  <si>
+    <t>Accès à l'application</t>
+  </si>
+  <si>
+    <t>Accès à l'application avec succès</t>
+  </si>
+  <si>
+    <t>Accès restreint lorsqu'on est pas connecté</t>
+  </si>
+  <si>
+    <t>Afficher des messages d'erreurs lorsque informations de connexion incorrectes</t>
+  </si>
+  <si>
+    <t>Échec de connexion</t>
+  </si>
+  <si>
+    <t>Échec avec succès</t>
+  </si>
+  <si>
+    <t>Reste sur la page de connexion</t>
+  </si>
+  <si>
+    <t>Reste sur la page de connexion avec succès</t>
+  </si>
+  <si>
+    <t>Bouton se souvenir de moi</t>
+  </si>
+  <si>
+    <t>Pas besoin de remplir à chaque fois ses identifiants</t>
+  </si>
+  <si>
+    <t>Succès</t>
+  </si>
+  <si>
+    <t>Se déconnecter</t>
+  </si>
+  <si>
+    <t>Être déconnecté</t>
+  </si>
+  <si>
+    <t>Stagiaires n'a accès qu'aux pages qui lui sont permises</t>
+  </si>
+  <si>
+    <t>Accès refusé s'il essaie d'accéder à une page à laquelle il n'a pas droit</t>
+  </si>
+  <si>
+    <t>Accès refusé avec succès</t>
+  </si>
+  <si>
+    <t>Enseignant n'a accès qu'aux pages qui lui sont permises</t>
+  </si>
+  <si>
+    <t>Maître de stage n'a accès qu'aux pages qui lui sont permises</t>
+  </si>
+  <si>
+    <t>Employeur n'a accès qu'aux pages qui lui sont permises</t>
+  </si>
+  <si>
+    <t>Coordonateur associe les utilisateurs à des rôles</t>
+  </si>
+  <si>
+    <t>Coordonateur peut supprimer chaque utilisateur</t>
+  </si>
+  <si>
+    <t>Coordonateur peut modifier chaque utilisateur</t>
+  </si>
+  <si>
+    <t>Coordonateur crée chaque utilisateur</t>
+  </si>
+  <si>
+    <t>Coordonateur peut relier ensemble enseignant et stagiaire</t>
+  </si>
+  <si>
+    <t>Coordonateur peut relier ensemble maître de stage s'il y a enseignant et stagiaire</t>
+  </si>
+  <si>
+    <t>Coordonateur peut modifier la liaison entre maître de stage et stagiaire</t>
+  </si>
+  <si>
+    <t>Coordonateur peut modifier la liaison entre enseignant et stagiaire</t>
+  </si>
+  <si>
+    <t>Utilisateur crée</t>
+  </si>
+  <si>
+    <t>Rôles associés</t>
+  </si>
+  <si>
+    <t>Utilisateur modifié</t>
+  </si>
+  <si>
+    <t>Utilisateur supprimé</t>
+  </si>
+  <si>
+    <t>Stagiaires-Enseignants associés</t>
+  </si>
+  <si>
+    <t>Maitre de stage associés</t>
+  </si>
+  <si>
+    <t>Liaison modifiée</t>
+  </si>
+  <si>
+    <t>Avec succès</t>
+  </si>
+  <si>
+    <t>Coordonateur a accès à la page de gestion des utilisateurs</t>
+  </si>
+  <si>
+    <t>Liste des utilisateurs</t>
+  </si>
+  <si>
+    <t>Coordonateur peut fournir des liens de connexion aux utilisateurs</t>
+  </si>
+  <si>
+    <t>Liens copiés</t>
+  </si>
+  <si>
+    <t>Pas encore implementé</t>
+  </si>
+  <si>
+    <t>Validation des champs de formulaires</t>
+  </si>
+  <si>
+    <t>Informations validées</t>
+  </si>
+  <si>
+    <t>Implementé, mais pas partout</t>
   </si>
 </sst>
 </file>
@@ -149,9 +318,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,14 +657,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDCE39D-6227-4181-9904-715834EED13D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C79B6EF-146B-4C68-8932-FB2A5C81FCD0}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="69.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.88671875" customWidth="1"/>
@@ -558,4 +730,640 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDCE39D-6227-4181-9904-715834EED13D}">
+  <dimension ref="A1:D75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="69.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="4" max="4" width="75.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout du manage pour l'employeur
</commit_message>
<xml_diff>
--- a/Tests/Plan_de_test_horaire.xlsx
+++ b/Tests/Plan_de_test_horaire.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Cegep\CegepSth\6_Session\PP\Gestion stagiaires SPU\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E06A3708-3BD1-4359-BF44-C30A66B75D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBD5E33-9AA6-4793-9EB9-9F6B83334414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{41F3187D-F1A2-49DE-9E3A-08B0683190F9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{41F3187D-F1A2-49DE-9E3A-08B0683190F9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Horaire" sheetId="1" r:id="rId1"/>
+    <sheet name="Horaire" sheetId="3" r:id="rId1"/>
+    <sheet name="Utilisateur" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>Tests</t>
   </si>
@@ -92,6 +93,174 @@
   </si>
   <si>
     <t>Ajouter une seule plage horaire qui est déjà prise.</t>
+  </si>
+  <si>
+    <t>Se connecter, stagiaire</t>
+  </si>
+  <si>
+    <t>Redirection vers la page d'accueil</t>
+  </si>
+  <si>
+    <t>Redirection vers la page d'accueil avec succès</t>
+  </si>
+  <si>
+    <t>Se connecter, coordonateur</t>
+  </si>
+  <si>
+    <t>Se connecter, maître de stage</t>
+  </si>
+  <si>
+    <t>Se connecter, employeur</t>
+  </si>
+  <si>
+    <t>Se connecter, enseignant</t>
+  </si>
+  <si>
+    <t>Redirection vers la page de gestion des utilisateurs</t>
+  </si>
+  <si>
+    <t>Redirection vers la page de gestion des utilisateurs avec succès</t>
+  </si>
+  <si>
+    <t>Redirection vers la page de gestion des maîtres de stages</t>
+  </si>
+  <si>
+    <t>Échec</t>
+  </si>
+  <si>
+    <t>Entrer les bonnes données de connexion</t>
+  </si>
+  <si>
+    <t>Accès à l'application</t>
+  </si>
+  <si>
+    <t>Accès à l'application avec succès</t>
+  </si>
+  <si>
+    <t>Accès restreint lorsqu'on est pas connecté</t>
+  </si>
+  <si>
+    <t>Afficher des messages d'erreurs lorsque informations de connexion incorrectes</t>
+  </si>
+  <si>
+    <t>Échec de connexion</t>
+  </si>
+  <si>
+    <t>Échec avec succès</t>
+  </si>
+  <si>
+    <t>Reste sur la page de connexion</t>
+  </si>
+  <si>
+    <t>Reste sur la page de connexion avec succès</t>
+  </si>
+  <si>
+    <t>Bouton se souvenir de moi</t>
+  </si>
+  <si>
+    <t>Pas besoin de remplir à chaque fois ses identifiants</t>
+  </si>
+  <si>
+    <t>Succès</t>
+  </si>
+  <si>
+    <t>Se déconnecter</t>
+  </si>
+  <si>
+    <t>Être déconnecté</t>
+  </si>
+  <si>
+    <t>Stagiaires n'a accès qu'aux pages qui lui sont permises</t>
+  </si>
+  <si>
+    <t>Accès refusé s'il essaie d'accéder à une page à laquelle il n'a pas droit</t>
+  </si>
+  <si>
+    <t>Accès refusé avec succès</t>
+  </si>
+  <si>
+    <t>Enseignant n'a accès qu'aux pages qui lui sont permises</t>
+  </si>
+  <si>
+    <t>Maître de stage n'a accès qu'aux pages qui lui sont permises</t>
+  </si>
+  <si>
+    <t>Employeur n'a accès qu'aux pages qui lui sont permises</t>
+  </si>
+  <si>
+    <t>Coordonateur associe les utilisateurs à des rôles</t>
+  </si>
+  <si>
+    <t>Coordonateur peut supprimer chaque utilisateur</t>
+  </si>
+  <si>
+    <t>Coordonateur peut modifier chaque utilisateur</t>
+  </si>
+  <si>
+    <t>Coordonateur crée chaque utilisateur</t>
+  </si>
+  <si>
+    <t>Coordonateur peut relier ensemble enseignant et stagiaire</t>
+  </si>
+  <si>
+    <t>Coordonateur peut relier ensemble maître de stage s'il y a enseignant et stagiaire</t>
+  </si>
+  <si>
+    <t>Coordonateur peut modifier la liaison entre maître de stage et stagiaire</t>
+  </si>
+  <si>
+    <t>Coordonateur peut modifier la liaison entre enseignant et stagiaire</t>
+  </si>
+  <si>
+    <t>Utilisateur crée</t>
+  </si>
+  <si>
+    <t>Rôles associés</t>
+  </si>
+  <si>
+    <t>Utilisateur modifié</t>
+  </si>
+  <si>
+    <t>Utilisateur supprimé</t>
+  </si>
+  <si>
+    <t>Stagiaires-Enseignants associés</t>
+  </si>
+  <si>
+    <t>Maitre de stage associés</t>
+  </si>
+  <si>
+    <t>Liaison modifiée</t>
+  </si>
+  <si>
+    <t>Avec succès</t>
+  </si>
+  <si>
+    <t>Coordonateur a accès à la page de gestion des utilisateurs</t>
+  </si>
+  <si>
+    <t>Liste des utilisateurs</t>
+  </si>
+  <si>
+    <t>Coordonateur peut fournir des liens de connexion aux utilisateurs</t>
+  </si>
+  <si>
+    <t>Liens copiés</t>
+  </si>
+  <si>
+    <t>Pas encore implementé</t>
+  </si>
+  <si>
+    <t>Validation des champs de formulaires</t>
+  </si>
+  <si>
+    <t>Informations validées</t>
+  </si>
+  <si>
+    <t>Implementé, mais pas partout</t>
+  </si>
+  <si>
+    <t>Redirection vers la page de gestion des stagiaires avec succès</t>
   </si>
 </sst>
 </file>
@@ -149,9 +318,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,14 +657,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDCE39D-6227-4181-9904-715834EED13D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C79B6EF-146B-4C68-8932-FB2A5C81FCD0}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="69.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.88671875" customWidth="1"/>
@@ -558,4 +730,638 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDCE39D-6227-4181-9904-715834EED13D}">
+  <dimension ref="A1:D75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="69.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="4" max="4" width="75.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ajout de tests pour la page d'horaire
</commit_message>
<xml_diff>
--- a/Tests/Plan_de_test_horaire.xlsx
+++ b/Tests/Plan_de_test_horaire.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Cegep\CegepSth\6_Session\PP\Gestion stagiaires SPU\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CEGEP\Hiver_2024\PRO\SPU\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12140E30-217E-436A-9EE6-185E6EF1C1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AA8964-556E-4A6B-9F23-30652DF27C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{41F3187D-F1A2-49DE-9E3A-08B0683190F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{41F3187D-F1A2-49DE-9E3A-08B0683190F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Horaire" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="90">
   <si>
     <t>Tests</t>
   </si>
@@ -261,6 +261,75 @@
   </si>
   <si>
     <t>Implementé, mais pas partout</t>
+  </si>
+  <si>
+    <t>Bouton affiché seulement pour les MDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encore des erreurs pour les stagiaires a accédé à la plage horaire si pas d'horaire associée donc n'a pas pu être testé </t>
+  </si>
+  <si>
+    <t>Échec de l'accès à la page</t>
+  </si>
+  <si>
+    <t>Plage horaire supprimée, retour à la page d'horaire</t>
+  </si>
+  <si>
+    <t>Retour à la page d'horaire, affichage du message d'erreur et la plage horaire n'est pas crée</t>
+  </si>
+  <si>
+    <t>Bouton inexistant pour les stagiaires</t>
+  </si>
+  <si>
+    <t>bouton visible et fonctionnel</t>
+  </si>
+  <si>
+    <t>Affichage de page de sélection d'horaire si MDS</t>
+  </si>
+  <si>
+    <t>Affichage de l'option d'ajout de plage horaire pour les MDS</t>
+  </si>
+  <si>
+    <t>Option d'ajout de plages horaire inexistant pour les stagiaires</t>
+  </si>
+  <si>
+    <t>Redirection a la page de sélection d'horaire</t>
+  </si>
+  <si>
+    <t>Redirection à la page d'horaire du stagiaire</t>
+  </si>
+  <si>
+    <t>Redirection a la page d'horaire avec message "aucun horaire assigné pour le moment"</t>
+  </si>
+  <si>
+    <t>Redirection du stagiaire à la page d'horaire avec un message indiquant aucun horaire si aucun ne lui est assignée</t>
+  </si>
+  <si>
+    <t>Redirection à l'horaire associé au stagiaire s'il en a un d'associé</t>
+  </si>
+  <si>
+    <t>Échec, affiche la page de sélection d'horaire</t>
+  </si>
+  <si>
+    <t>redirection en fonction du rôle n'est pas encore implémenté</t>
+  </si>
+  <si>
+    <t>Redirige à la page de sélection d'horaire</t>
+  </si>
+  <si>
+    <t>pas encore implémenté</t>
+  </si>
+  <si>
+    <t>Affichage du formulaire complet de modification de plage horaire en cliquant sur une plage horaire si MDS</t>
+  </si>
+  <si>
+    <t>Redirection vers le formulaire de modification de plage horaire</t>
+  </si>
+  <si>
+    <t>Affichage d'un pop-up demandant si on veut cocher absent ou non pour la plage horaire en cliquant sur la plage horaire si stagiaire</t>
+  </si>
+  <si>
+    <t>Affichage du pop-up swal qui demande a confirmer si on veut cocher l'absence</t>
   </si>
 </sst>
 </file>
@@ -658,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C79B6EF-146B-4C68-8932-FB2A5C81FCD0}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,44 +756,198 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -736,7 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDCE39D-6227-4181-9904-715834EED13D}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>